<commit_message>
updated pwd to new
</commit_message>
<xml_diff>
--- a/src/AVIS/TestData/AVIS_GUITestData_CreateReservation.xlsx
+++ b/src/AVIS/TestData/AVIS_GUITestData_CreateReservation.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GUI_Automation\selenium\GUI_TestDataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkhoday\git\ABG\src\AVIS\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView windowHeight="9735" windowWidth="24000" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Avis_GUI" sheetId="1" r:id="rId1"/>
-    <sheet name="Reservation_Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Avis_GUI" r:id="rId1" sheetId="1"/>
+    <sheet name="Reservation_Details" r:id="rId2" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Avis_GUI!$A$1:$AP$61</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Avis_GUI!$A$1:$AP$61</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
     <author>Doris Anto Pauline</author>
   </authors>
   <commentList>
-    <comment ref="R39" authorId="0" shapeId="0">
+    <comment authorId="0" ref="R39" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R51" authorId="0" shapeId="0">
+    <comment authorId="0" ref="R51" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="449">
   <si>
     <t>REGION</t>
   </si>
@@ -1033,9 +1033,6 @@
     <t/>
   </si>
   <si>
-    <t>Avis2018#</t>
-  </si>
-  <si>
     <t>INTERNET GUI</t>
   </si>
   <si>
@@ -1363,9 +1360,6 @@
     <t>$27.87</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Reservation created successfully. Reservation Number: 09899898US1</t>
   </si>
   <si>
@@ -1436,12 +1430,16 @@
   </si>
   <si>
     <t>09899940US1</t>
+  </si>
+  <si>
+    <t>Avis18nov$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1542,80 +1540,80 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="14" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1632,10 +1630,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1670,7 +1668,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1705,7 +1703,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1799,21 +1797,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1830,7 +1828,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1882,68 +1880,68 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="52.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="98.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="60.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="8.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6" style="3" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="28.140625" style="3" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="17.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="21" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="20.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="13.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="22.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="19.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="19.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="21.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="62.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="19.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="43" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="9.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="52.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="98.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="60.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="6.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="8.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="12.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="11.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="3" width="12.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="17" width="16.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="17" width="16.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="17" width="14.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="17" width="14.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="3" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="3" width="8.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="3" width="18.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="3" width="20.42578125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="8.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="6.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="3" width="28.140625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="3" width="17.28515625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="21.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="3" width="18.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="3" width="14.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="3" width="16.7109375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="3" width="20.5703125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="3" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="3" width="13.140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="3" width="13.7109375" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="3" width="14.0" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="3" width="22.85546875" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="3" width="19.5703125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" style="3" width="19.85546875" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" style="3" width="21.7109375" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="3" width="62.7109375" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" style="3" width="19.85546875" collapsed="true"/>
+    <col min="43" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row ht="15.75" r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1963,7 +1961,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>26</v>
@@ -2002,7 +2000,7 @@
         <v>43</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>46</v>
@@ -2079,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>17</v>
@@ -2091,7 +2089,7 @@
         <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>25</v>
@@ -2100,7 +2098,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>19</v>
@@ -2110,7 +2108,7 @@
       </c>
       <c r="M2" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="N2" s="28" t="s">
         <v>289</v>
@@ -2120,17 +2118,17 @@
       </c>
       <c r="P2" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R2" s="23" t="s">
         <v>291</v>
       </c>
       <c r="S2" s="25"/>
       <c r="T2" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U2" s="20" t="s">
         <v>52</v>
@@ -2150,13 +2148,13 @@
       <c r="Z2" s="25"/>
       <c r="AA2" s="25"/>
       <c r="AB2" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AC2" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="AD2" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>341</v>
       </c>
       <c r="AE2" s="6" t="s">
         <v>25</v>
@@ -2165,34 +2163,34 @@
         <v>25</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AH2" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AJ2" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN2" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="AK2" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL2" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM2" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="AP2" s="6" t="s">
         <v>415</v>
-      </c>
-      <c r="AO2" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="AP2" s="6" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
@@ -2203,7 +2201,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>17</v>
@@ -2215,7 +2213,7 @@
         <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>241</v>
@@ -2224,7 +2222,7 @@
         <v>18</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K3" s="23" t="s">
         <v>21</v>
@@ -2234,20 +2232,20 @@
       </c>
       <c r="M3" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O3" s="21" t="s">
         <v>241</v>
       </c>
       <c r="P3" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="R3" s="11" t="s">
         <v>295</v>
@@ -2270,7 +2268,7 @@
         <v>56</v>
       </c>
       <c r="Z3" s="16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AA3" s="16"/>
       <c r="AB3" s="6"/>
@@ -2297,7 +2295,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>17</v>
@@ -2309,7 +2307,7 @@
         <v>66</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H4" s="21" t="s">
         <v>241</v>
@@ -2318,7 +2316,7 @@
         <v>18</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>23</v>
@@ -2328,20 +2326,20 @@
       </c>
       <c r="M4" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>241</v>
       </c>
       <c r="P4" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q4" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="R4" s="11" t="s">
         <v>292</v>
@@ -2366,13 +2364,13 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
       <c r="AB4" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AC4" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="AD4" s="6" t="s">
         <v>352</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>353</v>
       </c>
       <c r="AE4" s="6" t="s">
         <v>241</v>
@@ -2381,34 +2379,34 @@
         <v>241</v>
       </c>
       <c r="AG4" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AH4" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AI4" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="AJ4" s="6" t="s">
+      <c r="AK4" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM4" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN4" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="AK4" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL4" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM4" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="AN4" s="6" t="s">
-        <v>357</v>
-      </c>
       <c r="AO4" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AP4" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
@@ -2419,7 +2417,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
@@ -2431,7 +2429,7 @@
         <v>68</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>242</v>
@@ -2440,7 +2438,7 @@
         <v>18</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>181</v>
@@ -2450,7 +2448,7 @@
       </c>
       <c r="M5" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "mm/dd/yy")</f>
-        <v>10/13/18</v>
+        <v>11/23/18</v>
       </c>
       <c r="N5" s="28" t="s">
         <v>51</v>
@@ -2460,10 +2458,10 @@
       </c>
       <c r="P5" s="24" t="str">
         <f ca="1">TEXT(TODAY()+5, "mm/dd/yy")</f>
-        <v>10/14/18</v>
+        <v>11/24/18</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="R5" s="11" t="s">
         <v>292</v>
@@ -2488,13 +2486,13 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="AC5" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="AC5" s="6" t="s">
-        <v>420</v>
-      </c>
       <c r="AD5" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AE5" s="6" t="s">
         <v>242</v>
@@ -2503,34 +2501,34 @@
         <v>242</v>
       </c>
       <c r="AG5" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="AH5" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="AH5" s="6" t="s">
+      <c r="AI5" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="AI5" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="AJ5" s="6" t="s">
+      <c r="AK5" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM5" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN5" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="AK5" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL5" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM5" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="AN5" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="AO5" s="6" t="s">
         <v>314</v>
       </c>
       <c r="AP5" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
@@ -2541,7 +2539,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -2553,7 +2551,7 @@
         <v>70</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>243</v>
@@ -2562,7 +2560,7 @@
         <v>18</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>183</v>
@@ -2572,7 +2570,7 @@
       </c>
       <c r="M6" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>288</v>
@@ -2582,7 +2580,7 @@
       </c>
       <c r="P6" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "mm/dd/yy")</f>
-        <v>10/13/18</v>
+        <v>11/23/18</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>288</v>
@@ -2612,13 +2610,13 @@
         <v>57</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AC6" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AE6" s="6" t="s">
         <v>243</v>
@@ -2627,34 +2625,34 @@
         <v>243</v>
       </c>
       <c r="AG6" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AH6" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AJ6" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AK6" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM6" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="AL6" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>346</v>
-      </c>
       <c r="AN6" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="AO6" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
@@ -2665,7 +2663,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
@@ -2677,7 +2675,7 @@
         <v>72</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>244</v>
@@ -2686,7 +2684,7 @@
         <v>18</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>185</v>
@@ -2696,7 +2694,7 @@
       </c>
       <c r="M7" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="N7" s="28" t="s">
         <v>286</v>
@@ -2706,7 +2704,7 @@
       </c>
       <c r="P7" s="24" t="str">
         <f ca="1">TEXT(TODAY()+5, "mm/dd/yy")</f>
-        <v>10/14/18</v>
+        <v>11/24/18</v>
       </c>
       <c r="Q7" s="4" t="s">
         <v>286</v>
@@ -2736,13 +2734,13 @@
       </c>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="AC7" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AE7" s="6" t="s">
         <v>244</v>
@@ -2751,34 +2749,34 @@
         <v>244</v>
       </c>
       <c r="AG7" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AH7" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AJ7" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="AK7" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AL7" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM7" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="AM7" s="6" t="s">
-        <v>346</v>
-      </c>
       <c r="AN7" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AO7" s="6" t="s">
         <v>314</v>
       </c>
       <c r="AP7" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
@@ -2789,7 +2787,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>17</v>
@@ -2801,7 +2799,7 @@
         <v>74</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>244</v>
@@ -2810,7 +2808,7 @@
         <v>18</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>187</v>
@@ -2820,7 +2818,7 @@
       </c>
       <c r="M8" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="N8" s="28" t="s">
         <v>286</v>
@@ -2830,7 +2828,7 @@
       </c>
       <c r="P8" s="24" t="str">
         <f ca="1">TEXT(TODAY()+5, "mm/dd/yy")</f>
-        <v>10/14/18</v>
+        <v>11/24/18</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>286</v>
@@ -2860,13 +2858,13 @@
         <v>310</v>
       </c>
       <c r="AB8" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AC8" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AD8" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AE8" s="6" t="s">
         <v>244</v>
@@ -2875,34 +2873,34 @@
         <v>244</v>
       </c>
       <c r="AG8" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AH8" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AI8" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AJ8" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AK8" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL8" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM8" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="AL8" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM8" s="6" t="s">
-        <v>346</v>
-      </c>
       <c r="AN8" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="AO8" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AP8" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
@@ -2913,7 +2911,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>17</v>
@@ -2925,7 +2923,7 @@
         <v>76</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>245</v>
@@ -2934,7 +2932,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>189</v>
@@ -2944,7 +2942,7 @@
       </c>
       <c r="M9" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="N9" s="28" t="s">
         <v>51</v>
@@ -2954,7 +2952,7 @@
       </c>
       <c r="P9" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "mm/dd/yy")</f>
-        <v>10/13/18</v>
+        <v>11/23/18</v>
       </c>
       <c r="Q9" s="4" t="s">
         <v>51</v>
@@ -2982,13 +2980,13 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AC9" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AD9" s="6" t="s">
         <v>439</v>
-      </c>
-      <c r="AC9" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>441</v>
       </c>
       <c r="AE9" s="6" t="s">
         <v>245</v>
@@ -2997,34 +2995,34 @@
         <v>245</v>
       </c>
       <c r="AG9" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AH9" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AI9" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AJ9" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="AK9" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL9" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM9" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="AL9" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM9" s="6" t="s">
-        <v>346</v>
-      </c>
       <c r="AN9" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="AO9" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="AP9" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
@@ -3035,7 +3033,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
@@ -3047,7 +3045,7 @@
         <v>78</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>246</v>
@@ -3056,7 +3054,7 @@
         <v>18</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>191</v>
@@ -3065,8 +3063,8 @@
         <v>192</v>
       </c>
       <c r="M10" s="24" t="str">
-        <f t="shared" ref="M10:M46" ca="1" si="0">TEXT(TODAY(), "mm/dd/yy")</f>
-        <v>10/09/18</v>
+        <f ca="1" ref="M10:M46" si="0" t="shared">TEXT(TODAY(), "mm/dd/yy")</f>
+        <v>11/19/18</v>
       </c>
       <c r="N10" s="28" t="s">
         <v>288</v>
@@ -3075,8 +3073,8 @@
         <v>246</v>
       </c>
       <c r="P10" s="24" t="str">
-        <f t="shared" ref="P10:P12" ca="1" si="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <f ca="1" ref="P10:P12" si="1" t="shared">TEXT(TODAY()+2, "mm/dd/yy")</f>
+        <v>11/21/18</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>288</v>
@@ -3104,13 +3102,13 @@
       <c r="Z10" s="6"/>
       <c r="AA10" s="6"/>
       <c r="AB10" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="AC10" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AD10" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="AD10" s="6" t="s">
-        <v>377</v>
       </c>
       <c r="AE10" s="6" t="s">
         <v>246</v>
@@ -3119,34 +3117,34 @@
         <v>246</v>
       </c>
       <c r="AG10" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AH10" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AI10" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AJ10" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="AK10" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL10" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM10" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN10" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="AK10" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL10" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM10" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="AN10" s="6" t="s">
-        <v>379</v>
-      </c>
       <c r="AO10" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="AP10" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
@@ -3157,7 +3155,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
@@ -3169,7 +3167,7 @@
         <v>80</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>247</v>
@@ -3178,7 +3176,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>193</v>
@@ -3187,8 +3185,8 @@
         <v>194</v>
       </c>
       <c r="M11" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N11" s="28" t="s">
         <v>288</v>
@@ -3197,11 +3195,11 @@
         <v>247</v>
       </c>
       <c r="P11" s="24" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>10/11/18</v>
+        <f ca="1" si="1" t="shared"/>
+        <v>11/21/18</v>
       </c>
       <c r="Q11" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R11" s="11" t="s">
         <v>292</v>
@@ -3226,13 +3224,13 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AC11" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AD11" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AE11" s="6" t="s">
         <v>247</v>
@@ -3241,34 +3239,34 @@
         <v>247</v>
       </c>
       <c r="AG11" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AH11" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AI11" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AJ11" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AK11" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL11" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM11" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN11" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="AK11" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL11" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM11" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="AN11" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="AO11" s="29" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AP11" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
@@ -3279,7 +3277,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>425</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>17</v>
@@ -3291,7 +3289,7 @@
         <v>82</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>248</v>
@@ -3300,7 +3298,7 @@
         <v>18</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>195</v>
@@ -3309,8 +3307,8 @@
         <v>196</v>
       </c>
       <c r="M12" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N12" s="28" t="s">
         <v>288</v>
@@ -3319,11 +3317,11 @@
         <v>248</v>
       </c>
       <c r="P12" s="24" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>10/11/18</v>
+        <f ca="1" si="1" t="shared"/>
+        <v>11/21/18</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R12" s="11" t="s">
         <v>291</v>
@@ -3348,13 +3346,13 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="AC12" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="AD12" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="AD12" s="6" t="s">
-        <v>341</v>
       </c>
       <c r="AE12" s="6" t="s">
         <v>248</v>
@@ -3363,31 +3361,31 @@
         <v>248</v>
       </c>
       <c r="AG12" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AH12" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="AI12" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="AJ12" s="6" t="s">
+      <c r="AK12" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL12" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM12" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN12" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="AK12" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL12" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM12" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="AN12" s="6" t="s">
-        <v>389</v>
-      </c>
       <c r="AO12" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="AP12" s="6"/>
     </row>
@@ -3411,7 +3409,7 @@
         <v>84</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>249</v>
@@ -3420,7 +3418,7 @@
         <v>18</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>197</v>
@@ -3430,7 +3428,7 @@
       </c>
       <c r="M13" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="N13" s="28" t="s">
         <v>288</v>
@@ -3440,7 +3438,7 @@
       </c>
       <c r="P13" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q13" s="4" t="s">
         <v>289</v>
@@ -3503,7 +3501,7 @@
         <v>86</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>250</v>
@@ -3512,7 +3510,7 @@
         <v>18</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K14" s="11" t="s">
         <v>199</v>
@@ -3522,7 +3520,7 @@
       </c>
       <c r="M14" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="N14" s="28" t="s">
         <v>288</v>
@@ -3532,10 +3530,10 @@
       </c>
       <c r="P14" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "mm/dd/yy")</f>
-        <v>10/13/18</v>
+        <v>11/23/18</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R14" s="11" t="s">
         <v>291</v>
@@ -3595,7 +3593,7 @@
         <v>88</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>251</v>
@@ -3604,7 +3602,7 @@
         <v>18</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K15" s="11" t="s">
         <v>201</v>
@@ -3613,8 +3611,8 @@
         <v>202</v>
       </c>
       <c r="M15" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N15" s="27" t="s">
         <v>286</v>
@@ -3624,7 +3622,7 @@
       </c>
       <c r="P15" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q15" s="4" t="s">
         <v>286</v>
@@ -3634,7 +3632,7 @@
       </c>
       <c r="S15" s="6"/>
       <c r="T15" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="U15" s="6" t="s">
         <v>54</v>
@@ -3691,7 +3689,7 @@
         <v>90</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>252</v>
@@ -3700,7 +3698,7 @@
         <v>18</v>
       </c>
       <c r="J16" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K16" s="11" t="s">
         <v>203</v>
@@ -3710,7 +3708,7 @@
       </c>
       <c r="M16" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="N16" s="27" t="s">
         <v>286</v>
@@ -3720,7 +3718,7 @@
       </c>
       <c r="P16" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "mm/dd/yy")</f>
-        <v>10/13/18</v>
+        <v>11/23/18</v>
       </c>
       <c r="Q16" s="4" t="s">
         <v>286</v>
@@ -3783,7 +3781,7 @@
         <v>92</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>253</v>
@@ -3792,7 +3790,7 @@
         <v>18</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>19</v>
@@ -3801,8 +3799,8 @@
         <v>20</v>
       </c>
       <c r="M17" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>286</v>
@@ -3812,7 +3810,7 @@
       </c>
       <c r="P17" s="24" t="str">
         <f ca="1">TEXT(TODAY(), "mm/dd/yy")</f>
-        <v>10/09/18</v>
+        <v>11/19/18</v>
       </c>
       <c r="Q17" s="5" t="s">
         <v>287</v>
@@ -3877,7 +3875,7 @@
         <v>94</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>254</v>
@@ -3886,7 +3884,7 @@
         <v>18</v>
       </c>
       <c r="J18" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>185</v>
@@ -3895,8 +3893,8 @@
         <v>186</v>
       </c>
       <c r="M18" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N18" s="5" t="s">
         <v>286</v>
@@ -3906,7 +3904,7 @@
       </c>
       <c r="P18" s="24" t="str">
         <f ca="1">TEXT(TODAY(), "mm/dd/yy")</f>
-        <v>10/09/18</v>
+        <v>11/19/18</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>286</v>
@@ -3969,7 +3967,7 @@
         <v>96</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>255</v>
@@ -3978,7 +3976,7 @@
         <v>18</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>205</v>
@@ -3987,8 +3985,8 @@
         <v>206</v>
       </c>
       <c r="M19" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N19" s="5" t="s">
         <v>286</v>
@@ -3998,7 +3996,7 @@
       </c>
       <c r="P19" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="Q19" s="5" t="s">
         <v>286</v>
@@ -4061,7 +4059,7 @@
         <v>98</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>256</v>
@@ -4070,7 +4068,7 @@
         <v>18</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K20" s="13" t="s">
         <v>207</v>
@@ -4079,8 +4077,8 @@
         <v>208</v>
       </c>
       <c r="M20" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N20" s="5" t="s">
         <v>286</v>
@@ -4090,7 +4088,7 @@
       </c>
       <c r="P20" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>286</v>
@@ -4153,7 +4151,7 @@
         <v>100</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>254</v>
@@ -4162,7 +4160,7 @@
         <v>18</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>209</v>
@@ -4171,8 +4169,8 @@
         <v>210</v>
       </c>
       <c r="M21" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N21" s="5" t="s">
         <v>286</v>
@@ -4182,7 +4180,7 @@
       </c>
       <c r="P21" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>286</v>
@@ -4245,7 +4243,7 @@
         <v>102</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>255</v>
@@ -4254,7 +4252,7 @@
         <v>18</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K22" s="13" t="s">
         <v>211</v>
@@ -4263,8 +4261,8 @@
         <v>212</v>
       </c>
       <c r="M22" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N22" s="5" t="s">
         <v>286</v>
@@ -4274,7 +4272,7 @@
       </c>
       <c r="P22" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <v>11/21/18</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>288</v>
@@ -4337,7 +4335,7 @@
         <v>104</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>257</v>
@@ -4346,7 +4344,7 @@
         <v>18</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K23" s="13" t="s">
         <v>213</v>
@@ -4355,8 +4353,8 @@
         <v>214</v>
       </c>
       <c r="M23" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N23" s="5" t="s">
         <v>286</v>
@@ -4366,7 +4364,7 @@
       </c>
       <c r="P23" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q23" s="5" t="s">
         <v>286</v>
@@ -4429,7 +4427,7 @@
         <v>106</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>256</v>
@@ -4438,7 +4436,7 @@
         <v>18</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K24" s="13" t="s">
         <v>215</v>
@@ -4447,8 +4445,8 @@
         <v>216</v>
       </c>
       <c r="M24" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N24" s="5" t="s">
         <v>286</v>
@@ -4458,7 +4456,7 @@
       </c>
       <c r="P24" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q24" s="5" t="s">
         <v>286</v>
@@ -4521,7 +4519,7 @@
         <v>108</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>257</v>
@@ -4530,7 +4528,7 @@
         <v>18</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K25" s="13" t="s">
         <v>217</v>
@@ -4539,8 +4537,8 @@
         <v>218</v>
       </c>
       <c r="M25" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N25" s="5" t="s">
         <v>286</v>
@@ -4550,7 +4548,7 @@
       </c>
       <c r="P25" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>289</v>
@@ -4603,7 +4601,7 @@
         <v>110</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>258</v>
@@ -4612,7 +4610,7 @@
         <v>18</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K26" s="13" t="s">
         <v>219</v>
@@ -4621,8 +4619,8 @@
         <v>220</v>
       </c>
       <c r="M26" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N26" s="5" t="s">
         <v>286</v>
@@ -4632,7 +4630,7 @@
       </c>
       <c r="P26" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "mm/dd/yy")</f>
-        <v>10/13/18</v>
+        <v>11/23/18</v>
       </c>
       <c r="Q26" s="5" t="s">
         <v>286</v>
@@ -4685,7 +4683,7 @@
         <v>112</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>259</v>
@@ -4694,7 +4692,7 @@
         <v>18</v>
       </c>
       <c r="J27" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K27" s="13" t="s">
         <v>221</v>
@@ -4703,8 +4701,8 @@
         <v>222</v>
       </c>
       <c r="M27" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N27" s="5" t="s">
         <v>286</v>
@@ -4714,7 +4712,7 @@
       </c>
       <c r="P27" s="24" t="str">
         <f ca="1">TEXT(TODAY()+6, "mm/dd/yy")</f>
-        <v>10/15/18</v>
+        <v>11/25/18</v>
       </c>
       <c r="Q27" s="5" t="s">
         <v>286</v>
@@ -4767,7 +4765,7 @@
         <v>114</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>260</v>
@@ -4776,7 +4774,7 @@
         <v>18</v>
       </c>
       <c r="J28" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K28" s="13" t="s">
         <v>223</v>
@@ -4785,8 +4783,8 @@
         <v>224</v>
       </c>
       <c r="M28" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N28" s="5" t="s">
         <v>286</v>
@@ -4796,7 +4794,7 @@
       </c>
       <c r="P28" s="24" t="str">
         <f ca="1">TEXT(TODAY()+7, "mm/dd/yy")</f>
-        <v>10/16/18</v>
+        <v>11/26/18</v>
       </c>
       <c r="Q28" s="5" t="s">
         <v>288</v>
@@ -4849,7 +4847,7 @@
         <v>116</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>261</v>
@@ -4858,7 +4856,7 @@
         <v>18</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K29" s="13" t="s">
         <v>225</v>
@@ -4867,8 +4865,8 @@
         <v>226</v>
       </c>
       <c r="M29" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N29" s="5" t="s">
         <v>286</v>
@@ -4878,7 +4876,7 @@
       </c>
       <c r="P29" s="24" t="str">
         <f ca="1">TEXT(TODAY()+66, "mm/dd/yy")</f>
-        <v>12/14/18</v>
+        <v>01/24/19</v>
       </c>
       <c r="Q29" s="5" t="s">
         <v>286</v>
@@ -4931,7 +4929,7 @@
         <v>118</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>262</v>
@@ -4940,7 +4938,7 @@
         <v>18</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K30" s="13" t="s">
         <v>227</v>
@@ -4949,8 +4947,8 @@
         <v>228</v>
       </c>
       <c r="M30" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N30" s="5" t="s">
         <v>286</v>
@@ -4960,7 +4958,7 @@
       </c>
       <c r="P30" s="24" t="str">
         <f ca="1">TEXT(TODAY()+54, "mm/dd/yy")</f>
-        <v>12/02/18</v>
+        <v>01/12/19</v>
       </c>
       <c r="Q30" s="5" t="s">
         <v>286</v>
@@ -5013,7 +5011,7 @@
         <v>120</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>263</v>
@@ -5022,7 +5020,7 @@
         <v>18</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K31" s="13" t="s">
         <v>229</v>
@@ -5031,8 +5029,8 @@
         <v>230</v>
       </c>
       <c r="M31" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N31" s="5" t="s">
         <v>286</v>
@@ -5042,7 +5040,7 @@
       </c>
       <c r="P31" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="Q31" s="5" t="s">
         <v>286</v>
@@ -5095,7 +5093,7 @@
         <v>122</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>264</v>
@@ -5104,7 +5102,7 @@
         <v>18</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K32" s="11" t="s">
         <v>19</v>
@@ -5113,8 +5111,8 @@
         <v>20</v>
       </c>
       <c r="M32" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N32" s="27" t="s">
         <v>289</v>
@@ -5124,17 +5122,17 @@
       </c>
       <c r="P32" s="24" t="str">
         <f ca="1">TEXT(TODAY(), "mm/dd/yy")</f>
-        <v>10/09/18</v>
+        <v>11/19/18</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R32" s="11" t="s">
         <v>290</v>
       </c>
       <c r="S32" s="6"/>
       <c r="T32" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="U32" s="7" t="s">
         <v>52</v>
@@ -5189,7 +5187,7 @@
         <v>124</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>265</v>
@@ -5198,7 +5196,7 @@
         <v>18</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K33" s="11" t="s">
         <v>23</v>
@@ -5207,8 +5205,8 @@
         <v>24</v>
       </c>
       <c r="M33" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N33" s="27" t="s">
         <v>288</v>
@@ -5218,7 +5216,7 @@
       </c>
       <c r="P33" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="Q33" s="4" t="s">
         <v>288</v>
@@ -5281,7 +5279,7 @@
         <v>126</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>266</v>
@@ -5290,7 +5288,7 @@
         <v>18</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K34" s="11" t="s">
         <v>181</v>
@@ -5299,8 +5297,8 @@
         <v>182</v>
       </c>
       <c r="M34" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N34" s="27" t="s">
         <v>286</v>
@@ -5310,10 +5308,10 @@
       </c>
       <c r="P34" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R34" s="11" t="s">
         <v>292</v>
@@ -5373,7 +5371,7 @@
         <v>128</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>267</v>
@@ -5382,7 +5380,7 @@
         <v>18</v>
       </c>
       <c r="J35" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K35" s="11" t="s">
         <v>183</v>
@@ -5391,8 +5389,8 @@
         <v>184</v>
       </c>
       <c r="M35" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N35" s="27" t="s">
         <v>288</v>
@@ -5402,7 +5400,7 @@
       </c>
       <c r="P35" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="Q35" s="4" t="s">
         <v>288</v>
@@ -5465,7 +5463,7 @@
         <v>130</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>268</v>
@@ -5474,7 +5472,7 @@
         <v>18</v>
       </c>
       <c r="J36" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K36" s="11" t="s">
         <v>229</v>
@@ -5483,8 +5481,8 @@
         <v>230</v>
       </c>
       <c r="M36" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N36" s="27" t="s">
         <v>288</v>
@@ -5494,7 +5492,7 @@
       </c>
       <c r="P36" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "mm/dd/yy")</f>
-        <v>10/10/18</v>
+        <v>11/20/18</v>
       </c>
       <c r="Q36" s="4" t="s">
         <v>288</v>
@@ -5557,7 +5555,7 @@
         <v>132</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>269</v>
@@ -5566,7 +5564,7 @@
         <v>18</v>
       </c>
       <c r="J37" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K37" s="11" t="s">
         <v>187</v>
@@ -5575,8 +5573,8 @@
         <v>188</v>
       </c>
       <c r="M37" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N37" s="27" t="s">
         <v>288</v>
@@ -5585,8 +5583,8 @@
         <v>269</v>
       </c>
       <c r="P37" s="24" t="str">
-        <f t="shared" ref="P37:P42" ca="1" si="2">TEXT(TODAY()+2, "mm/dd/yy")</f>
-        <v>10/11/18</v>
+        <f ca="1" ref="P37:P42" si="2" t="shared">TEXT(TODAY()+2, "mm/dd/yy")</f>
+        <v>11/21/18</v>
       </c>
       <c r="Q37" s="4" t="s">
         <v>51</v>
@@ -5649,7 +5647,7 @@
         <v>134</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>264</v>
@@ -5658,7 +5656,7 @@
         <v>18</v>
       </c>
       <c r="J38" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K38" s="11" t="s">
         <v>191</v>
@@ -5667,8 +5665,8 @@
         <v>192</v>
       </c>
       <c r="M38" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N38" s="27" t="s">
         <v>288</v>
@@ -5677,8 +5675,8 @@
         <v>264</v>
       </c>
       <c r="P38" s="24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>10/11/18</v>
+        <f ca="1" si="2" t="shared"/>
+        <v>11/21/18</v>
       </c>
       <c r="Q38" s="4" t="s">
         <v>288</v>
@@ -5741,7 +5739,7 @@
         <v>136</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>268</v>
@@ -5750,7 +5748,7 @@
         <v>18</v>
       </c>
       <c r="J39" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K39" s="11" t="s">
         <v>193</v>
@@ -5759,8 +5757,8 @@
         <v>194</v>
       </c>
       <c r="M39" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N39" s="27" t="s">
         <v>288</v>
@@ -5769,11 +5767,11 @@
         <v>268</v>
       </c>
       <c r="P39" s="24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>10/11/18</v>
+        <f ca="1" si="2" t="shared"/>
+        <v>11/21/18</v>
       </c>
       <c r="Q39" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R39" s="11" t="s">
         <v>294</v>
@@ -5833,7 +5831,7 @@
         <v>138</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>265</v>
@@ -5842,7 +5840,7 @@
         <v>18</v>
       </c>
       <c r="J40" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K40" s="11" t="s">
         <v>195</v>
@@ -5851,8 +5849,8 @@
         <v>196</v>
       </c>
       <c r="M40" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N40" s="27" t="s">
         <v>288</v>
@@ -5861,11 +5859,11 @@
         <v>265</v>
       </c>
       <c r="P40" s="24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>10/11/18</v>
+        <f ca="1" si="2" t="shared"/>
+        <v>11/21/18</v>
       </c>
       <c r="Q40" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R40" s="11" t="s">
         <v>291</v>
@@ -5915,7 +5913,7 @@
         <v>140</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>266</v>
@@ -5924,7 +5922,7 @@
         <v>18</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K41" s="11" t="s">
         <v>197</v>
@@ -5933,8 +5931,8 @@
         <v>198</v>
       </c>
       <c r="M41" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N41" s="27" t="s">
         <v>288</v>
@@ -5943,8 +5941,8 @@
         <v>266</v>
       </c>
       <c r="P41" s="24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>10/11/18</v>
+        <f ca="1" si="2" t="shared"/>
+        <v>11/21/18</v>
       </c>
       <c r="Q41" s="4" t="s">
         <v>289</v>
@@ -5954,7 +5952,7 @@
       </c>
       <c r="S41" s="6"/>
       <c r="T41" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="U41" s="7"/>
       <c r="V41" s="6"/>
@@ -5999,7 +5997,7 @@
         <v>142</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>267</v>
@@ -6008,7 +6006,7 @@
         <v>18</v>
       </c>
       <c r="J42" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K42" s="11" t="s">
         <v>199</v>
@@ -6017,8 +6015,8 @@
         <v>200</v>
       </c>
       <c r="M42" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N42" s="27" t="s">
         <v>288</v>
@@ -6027,18 +6025,18 @@
         <v>267</v>
       </c>
       <c r="P42" s="24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>10/11/18</v>
+        <f ca="1" si="2" t="shared"/>
+        <v>11/21/18</v>
       </c>
       <c r="Q42" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R42" s="11" t="s">
         <v>291</v>
       </c>
       <c r="S42" s="6"/>
       <c r="T42" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="U42" s="6"/>
       <c r="V42" s="7"/>
@@ -6083,7 +6081,7 @@
         <v>144</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>268</v>
@@ -6092,7 +6090,7 @@
         <v>18</v>
       </c>
       <c r="J43" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K43" s="11" t="s">
         <v>201</v>
@@ -6101,8 +6099,8 @@
         <v>202</v>
       </c>
       <c r="M43" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N43" s="27" t="s">
         <v>286</v>
@@ -6112,7 +6110,7 @@
       </c>
       <c r="P43" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q43" s="4" t="s">
         <v>286</v>
@@ -6122,7 +6120,7 @@
       </c>
       <c r="S43" s="6"/>
       <c r="T43" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
@@ -6167,7 +6165,7 @@
         <v>146</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>270</v>
@@ -6176,7 +6174,7 @@
         <v>18</v>
       </c>
       <c r="J44" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K44" s="11" t="s">
         <v>203</v>
@@ -6185,8 +6183,8 @@
         <v>204</v>
       </c>
       <c r="M44" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N44" s="27" t="s">
         <v>286</v>
@@ -6196,7 +6194,7 @@
       </c>
       <c r="P44" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q44" s="4" t="s">
         <v>286</v>
@@ -6206,7 +6204,7 @@
       </c>
       <c r="S44" s="6"/>
       <c r="T44" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
@@ -6251,7 +6249,7 @@
         <v>148</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H45" s="12" t="s">
         <v>265</v>
@@ -6260,7 +6258,7 @@
         <v>18</v>
       </c>
       <c r="J45" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K45" s="11" t="s">
         <v>231</v>
@@ -6269,8 +6267,8 @@
         <v>232</v>
       </c>
       <c r="M45" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N45" s="27" t="s">
         <v>288</v>
@@ -6280,10 +6278,10 @@
       </c>
       <c r="P45" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q45" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R45" s="11" t="s">
         <v>291</v>
@@ -6332,7 +6330,7 @@
         <v>150</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H46" s="12" t="s">
         <v>271</v>
@@ -6341,7 +6339,7 @@
         <v>18</v>
       </c>
       <c r="J46" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K46" s="15" t="s">
         <v>233</v>
@@ -6350,8 +6348,8 @@
         <v>234</v>
       </c>
       <c r="M46" s="24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>10/09/18</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>11/19/18</v>
       </c>
       <c r="N46" s="27" t="s">
         <v>288</v>
@@ -6361,7 +6359,7 @@
       </c>
       <c r="P46" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "mm/dd/yy")</f>
-        <v>10/12/18</v>
+        <v>11/22/18</v>
       </c>
       <c r="Q46" s="4" t="s">
         <v>51</v>
@@ -6371,7 +6369,7 @@
       </c>
       <c r="S46" s="6"/>
       <c r="T46" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
@@ -6416,7 +6414,7 @@
         <v>152</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>272</v>
@@ -6425,7 +6423,7 @@
         <v>18</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K47" s="11" t="s">
         <v>21</v>
@@ -6435,7 +6433,7 @@
       </c>
       <c r="M47" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "dd/mm/yy")</f>
-        <v>10/10/18</v>
+        <v>20/11/18</v>
       </c>
       <c r="N47" s="27" t="s">
         <v>51</v>
@@ -6445,10 +6443,10 @@
       </c>
       <c r="P47" s="24" t="str">
         <f ca="1">TEXT(TODAY()+1, "dd/mm/yy")</f>
-        <v>10/10/18</v>
+        <v>20/11/18</v>
       </c>
       <c r="Q47" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R47" s="11" t="s">
         <v>290</v>
@@ -6471,7 +6469,7 @@
         <v>56</v>
       </c>
       <c r="Z47" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AA47" s="6"/>
       <c r="AB47" s="6"/>
@@ -6510,7 +6508,7 @@
         <v>154</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H48" s="12" t="s">
         <v>273</v>
@@ -6519,7 +6517,7 @@
         <v>18</v>
       </c>
       <c r="J48" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K48" s="11" t="s">
         <v>183</v>
@@ -6528,8 +6526,8 @@
         <v>184</v>
       </c>
       <c r="M48" s="24" t="str">
-        <f t="shared" ref="M48:M61" ca="1" si="3">TEXT(TODAY()+1, "dd/mm/yy")</f>
-        <v>10/10/18</v>
+        <f ca="1" ref="M48:M61" si="3" t="shared">TEXT(TODAY()+1, "dd/mm/yy")</f>
+        <v>20/11/18</v>
       </c>
       <c r="N48" s="27" t="s">
         <v>288</v>
@@ -6539,7 +6537,7 @@
       </c>
       <c r="P48" s="24" t="str">
         <f ca="1">TEXT(TODAY()+2, "dd/mm/yy")</f>
-        <v>11/10/18</v>
+        <v>21/11/18</v>
       </c>
       <c r="Q48" s="4" t="s">
         <v>288</v>
@@ -6602,7 +6600,7 @@
         <v>156</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>274</v>
@@ -6611,7 +6609,7 @@
         <v>18</v>
       </c>
       <c r="J49" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K49" s="11" t="s">
         <v>187</v>
@@ -6620,8 +6618,8 @@
         <v>188</v>
       </c>
       <c r="M49" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N49" s="27" t="s">
         <v>288</v>
@@ -6631,7 +6629,7 @@
       </c>
       <c r="P49" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "dd/mm/yy")</f>
-        <v>12/10/18</v>
+        <v>22/11/18</v>
       </c>
       <c r="Q49" s="27" t="s">
         <v>288</v>
@@ -6694,7 +6692,7 @@
         <v>158</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>275</v>
@@ -6703,7 +6701,7 @@
         <v>18</v>
       </c>
       <c r="J50" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K50" s="11" t="s">
         <v>191</v>
@@ -6712,8 +6710,8 @@
         <v>192</v>
       </c>
       <c r="M50" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N50" s="27" t="s">
         <v>288</v>
@@ -6723,7 +6721,7 @@
       </c>
       <c r="P50" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "dd/mm/yy")</f>
-        <v>12/10/18</v>
+        <v>22/11/18</v>
       </c>
       <c r="Q50" s="4" t="s">
         <v>288</v>
@@ -6786,7 +6784,7 @@
         <v>160</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H51" s="12" t="s">
         <v>276</v>
@@ -6795,7 +6793,7 @@
         <v>18</v>
       </c>
       <c r="J51" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K51" s="11" t="s">
         <v>193</v>
@@ -6804,8 +6802,8 @@
         <v>194</v>
       </c>
       <c r="M51" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N51" s="27" t="s">
         <v>288</v>
@@ -6815,10 +6813,10 @@
       </c>
       <c r="P51" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "dd/mm/yy")</f>
-        <v>12/10/18</v>
+        <v>22/11/18</v>
       </c>
       <c r="Q51" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R51" s="11" t="s">
         <v>294</v>
@@ -6878,7 +6876,7 @@
         <v>162</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H52" s="12" t="s">
         <v>277</v>
@@ -6887,7 +6885,7 @@
         <v>18</v>
       </c>
       <c r="J52" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K52" s="11" t="s">
         <v>195</v>
@@ -6896,8 +6894,8 @@
         <v>196</v>
       </c>
       <c r="M52" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N52" s="27" t="s">
         <v>288</v>
@@ -6907,10 +6905,10 @@
       </c>
       <c r="P52" s="24" t="str">
         <f ca="1">TEXT(TODAY()+3, "dd/mm/yy")</f>
-        <v>12/10/18</v>
+        <v>22/11/18</v>
       </c>
       <c r="Q52" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R52" s="11" t="s">
         <v>291</v>
@@ -6970,7 +6968,7 @@
         <v>164</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>278</v>
@@ -6979,7 +6977,7 @@
         <v>18</v>
       </c>
       <c r="J53" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K53" s="11" t="s">
         <v>201</v>
@@ -6988,8 +6986,8 @@
         <v>202</v>
       </c>
       <c r="M53" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N53" s="27" t="s">
         <v>286</v>
@@ -6999,7 +6997,7 @@
       </c>
       <c r="P53" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "dd/mm/yy")</f>
-        <v>13/10/18</v>
+        <v>23/11/18</v>
       </c>
       <c r="Q53" s="4" t="s">
         <v>286</v>
@@ -7062,7 +7060,7 @@
         <v>166</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>273</v>
@@ -7071,7 +7069,7 @@
         <v>18</v>
       </c>
       <c r="J54" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K54" s="11" t="s">
         <v>203</v>
@@ -7080,8 +7078,8 @@
         <v>204</v>
       </c>
       <c r="M54" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N54" s="27" t="s">
         <v>286</v>
@@ -7091,7 +7089,7 @@
       </c>
       <c r="P54" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "dd/mm/yy")</f>
-        <v>13/10/18</v>
+        <v>23/11/18</v>
       </c>
       <c r="Q54" s="4" t="s">
         <v>286</v>
@@ -7154,7 +7152,7 @@
         <v>168</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>279</v>
@@ -7163,7 +7161,7 @@
         <v>18</v>
       </c>
       <c r="J55" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K55" s="11" t="s">
         <v>231</v>
@@ -7172,8 +7170,8 @@
         <v>232</v>
       </c>
       <c r="M55" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N55" s="27" t="s">
         <v>288</v>
@@ -7183,10 +7181,10 @@
       </c>
       <c r="P55" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "dd/mm/yy")</f>
-        <v>13/10/18</v>
+        <v>23/11/18</v>
       </c>
       <c r="Q55" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R55" s="11" t="s">
         <v>291</v>
@@ -7236,7 +7234,7 @@
         <v>170</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>280</v>
@@ -7245,7 +7243,7 @@
         <v>18</v>
       </c>
       <c r="J56" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K56" s="15" t="s">
         <v>233</v>
@@ -7254,8 +7252,8 @@
         <v>234</v>
       </c>
       <c r="M56" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N56" s="27" t="s">
         <v>288</v>
@@ -7265,7 +7263,7 @@
       </c>
       <c r="P56" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "dd/mm/yy")</f>
-        <v>13/10/18</v>
+        <v>23/11/18</v>
       </c>
       <c r="Q56" s="4" t="s">
         <v>51</v>
@@ -7318,7 +7316,7 @@
         <v>172</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>281</v>
@@ -7327,7 +7325,7 @@
         <v>18</v>
       </c>
       <c r="J57" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K57" s="15" t="s">
         <v>235</v>
@@ -7336,8 +7334,8 @@
         <v>236</v>
       </c>
       <c r="M57" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>288</v>
@@ -7347,10 +7345,10 @@
       </c>
       <c r="P57" s="24" t="str">
         <f ca="1">TEXT(TODAY()+4, "dd/mm/yy")</f>
-        <v>13/10/18</v>
+        <v>23/11/18</v>
       </c>
       <c r="Q57" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R57" s="11" t="s">
         <v>294</v>
@@ -7400,7 +7398,7 @@
         <v>174</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>282</v>
@@ -7409,7 +7407,7 @@
         <v>18</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K58" s="15" t="s">
         <v>213</v>
@@ -7418,8 +7416,8 @@
         <v>214</v>
       </c>
       <c r="M58" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>286</v>
@@ -7429,7 +7427,7 @@
       </c>
       <c r="P58" s="24" t="str">
         <f ca="1">TEXT(TODAY()+5, "dd/mm/yy")</f>
-        <v>14/10/18</v>
+        <v>24/11/18</v>
       </c>
       <c r="Q58" s="4" t="s">
         <v>286</v>
@@ -7482,7 +7480,7 @@
         <v>176</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>283</v>
@@ -7491,7 +7489,7 @@
         <v>18</v>
       </c>
       <c r="J59" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K59" s="11" t="s">
         <v>223</v>
@@ -7500,8 +7498,8 @@
         <v>224</v>
       </c>
       <c r="M59" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N59" s="4" t="s">
         <v>288</v>
@@ -7511,7 +7509,7 @@
       </c>
       <c r="P59" s="24" t="str">
         <f ca="1">TEXT(TODAY()+5, "dd/mm/yy")</f>
-        <v>14/10/18</v>
+        <v>24/11/18</v>
       </c>
       <c r="Q59" s="4" t="s">
         <v>288</v>
@@ -7564,7 +7562,7 @@
         <v>178</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>284</v>
@@ -7573,7 +7571,7 @@
         <v>18</v>
       </c>
       <c r="J60" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K60" s="11" t="s">
         <v>237</v>
@@ -7582,8 +7580,8 @@
         <v>238</v>
       </c>
       <c r="M60" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N60" s="4" t="s">
         <v>288</v>
@@ -7593,7 +7591,7 @@
       </c>
       <c r="P60" s="24" t="str">
         <f ca="1">TEXT(TODAY()+5, "dd/mm/yy")</f>
-        <v>14/10/18</v>
+        <v>24/11/18</v>
       </c>
       <c r="Q60" s="4" t="s">
         <v>288</v>
@@ -7646,7 +7644,7 @@
         <v>180</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>285</v>
@@ -7655,7 +7653,7 @@
         <v>18</v>
       </c>
       <c r="J61" s="22" t="s">
-        <v>315</v>
+        <v>448</v>
       </c>
       <c r="K61" s="11" t="s">
         <v>239</v>
@@ -7664,8 +7662,8 @@
         <v>240</v>
       </c>
       <c r="M61" s="24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>10/10/18</v>
+        <f ca="1" si="3" t="shared"/>
+        <v>20/11/18</v>
       </c>
       <c r="N61" s="4" t="s">
         <v>288</v>
@@ -7675,10 +7673,10 @@
       </c>
       <c r="P61" s="24" t="str">
         <f ca="1">TEXT(TODAY()+5, "dd/mm/yy")</f>
-        <v>14/10/18</v>
+        <v>24/11/18</v>
       </c>
       <c r="Q61" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="R61" s="11" t="s">
         <v>292</v>
@@ -7797,15 +7795,15 @@
       <c r="AP63" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
@@ -7813,24 +7811,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="63.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="63.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row ht="15.75" r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -7897,16 +7895,16 @@
         <v>43381</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>341</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>25</v>
@@ -7915,31 +7913,31 @@
         <v>25</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>347</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -7947,13 +7945,13 @@
         <v>43381</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C3" s="32">
         <v>43381</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -7975,22 +7973,22 @@
         <v>43381</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C4" s="32">
         <v>43384</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>352</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>353</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>241</v>
@@ -7999,31 +7997,31 @@
         <v>241</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>357</v>
-      </c>
       <c r="R4" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -8037,16 +8035,16 @@
         <v>43384</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>242</v>
@@ -8055,31 +8053,31 @@
         <v>242</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>355</v>
-      </c>
       <c r="M5" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>361</v>
-      </c>
       <c r="R5" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -8126,13 +8124,13 @@
         <v>286</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>244</v>
@@ -8141,31 +8139,31 @@
         <v>244</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K7" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q7" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="O7" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>368</v>
-      </c>
       <c r="R7" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -8212,13 +8210,13 @@
         <v>51</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>370</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>371</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>245</v>
@@ -8227,31 +8225,31 @@
         <v>245</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K9" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>365</v>
-      </c>
       <c r="M9" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q9" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>373</v>
-      </c>
       <c r="R9" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -8268,13 +8266,13 @@
         <v>288</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>377</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>246</v>
@@ -8283,31 +8281,31 @@
         <v>246</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K10" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>365</v>
-      </c>
       <c r="M10" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q10" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>379</v>
-      </c>
       <c r="R10" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -8321,16 +8319,16 @@
         <v>43385</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>382</v>
-      </c>
       <c r="G11" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>247</v>
@@ -8339,54 +8337,54 @@
         <v>247</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K11" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>365</v>
-      </c>
       <c r="M11" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q11" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="N11" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="R11" s="29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>288</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F12" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>341</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>248</v>
@@ -8395,54 +8393,54 @@
         <v>248</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K12" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="L12" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="M12" s="6" t="s">
+      <c r="N12" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q12" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>389</v>
-      </c>
       <c r="R12" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>288</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>289</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>249</v>
@@ -8451,54 +8449,54 @@
         <v>249</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L13" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="M13" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="N13" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q13" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="N13" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>394</v>
-      </c>
       <c r="R13" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>288</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>397</v>
-      </c>
       <c r="G14" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>250</v>
@@ -8507,54 +8505,54 @@
         <v>250</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M14" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q14" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>399</v>
-      </c>
       <c r="R14" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>286</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>286</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>251</v>
@@ -8563,54 +8561,54 @@
         <v>251</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K15" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="N15" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="O15" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q15" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="O15" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>406</v>
-      </c>
       <c r="R15" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>286</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>286</v>
       </c>
       <c r="E16" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>407</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>408</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>252</v>
@@ -8619,35 +8617,35 @@
         <v>252</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K16" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>403</v>
-      </c>
       <c r="M16" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q16" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="N16" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q16" s="6" t="s">
+      <c r="R16" s="6" t="s">
         <v>410</v>
-      </c>
-      <c r="R16" s="6" t="s">
-        <v>411</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>